<commit_message>
Some work off of south Musky Lake Rd
</commit_message>
<xml_diff>
--- a/Bayfield County/Data/Trail Mapping Info.xlsx
+++ b/Bayfield County/Data/Trail Mapping Info.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aaaPersonal\Maps_GPS\Bayfield County\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aaaPersonal\MAPPING\Bayfield County\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11148" windowHeight="9000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tracks" sheetId="1" r:id="rId1"/>
@@ -2955,9 +2955,9 @@
   </sheetPr>
   <dimension ref="A1:Y268"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I98" sqref="I98"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9785,9 +9785,9 @@
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>